<commit_message>
turning off district heat boolean, suppressing lignite+ccs, coal+ccs, and biomass+ccs
</commit_message>
<xml_diff>
--- a/InputData/elec/BBPPRTY/BAU Ban Power Plant Retrofits This Year.xlsx
+++ b/InputData/elec/BBPPRTY/BAU Ban Power Plant Retrofits This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\BBPPRTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\EPS Models\EU EPS\InputData\elec\BBPPRTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B110B6C9-74C0-49E9-BE6A-2B50706FF589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F17E2C0-D048-4518-95D6-DE39D9AFD468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34665" yWindow="3195" windowWidth="19830" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2955" yWindow="2085" windowWidth="22425" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -508,48 +508,48 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.81640625" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -567,17 +567,17 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:AE22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -672,7 +672,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2287,102 +2287,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2477,197 +2477,197 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>

</xml_diff>